<commit_message>
q7 finished with chart question
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\d10\Projects\lookups-budget-seanmalley1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC275D6-5E64-4E6A-A509-71BCDC1AC739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B77E25D-2C3C-464B-AF19-008623D1B47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45972" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="94">
   <si>
     <t>Department</t>
   </si>
@@ -335,6 +335,9 @@
   </si>
   <si>
     <t>FY19_diff_V2</t>
+  </si>
+  <si>
+    <t>ASK HOW TO CHANGE SERIES TO BUDGET/</t>
   </si>
 </sst>
 </file>
@@ -946,6 +949,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Fiscal Year Differences by Dept</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -982,8 +1010,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.20968959247034449"/>
-          <c:y val="4.2083333333333355E-2"/>
+          <c:x val="0.19973061301092629"/>
+          <c:y val="3.0910603194354156E-2"/>
           <c:w val="0.79031040752965553"/>
           <c:h val="0.61498432487605714"/>
         </c:manualLayout>
@@ -1850,16 +1878,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>290407</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>52917</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>184816</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>49410</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1082039</xdr:colOff>
-      <xdr:row>97</xdr:row>
-      <xdr:rowOff>52917</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>973425</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>85393</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2186,8 +2214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74:E79"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K81" sqref="K81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -5406,7 +5434,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A65" t="s">
         <v>24</v>
       </c>
@@ -5423,7 +5451,7 @@
         <v>-9181.0800000000163</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A66" t="s">
         <v>25</v>
       </c>
@@ -5440,7 +5468,7 @@
         <v>-311228.08999999997</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A67" t="s">
         <v>32</v>
       </c>
@@ -5457,7 +5485,7 @@
         <v>-374962.91000000015</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A68" t="s">
         <v>38</v>
       </c>
@@ -5474,7 +5502,7 @@
         <v>-72.879999999888241</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A69" t="s">
         <v>39</v>
       </c>
@@ -5491,7 +5519,7 @@
         <v>-1724.9000000000233</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A70" t="s">
         <v>55</v>
       </c>
@@ -5508,12 +5536,12 @@
         <v>-82077.349999999627</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A72" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -5536,7 +5564,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A74" t="s">
         <v>24</v>
       </c>
@@ -5565,7 +5593,7 @@
         <v>-9181.0800000000163</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A75" t="s">
         <v>25</v>
       </c>
@@ -5594,7 +5622,7 @@
         <v>-311228.08999999997</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A76" t="s">
         <v>32</v>
       </c>
@@ -5623,7 +5651,7 @@
         <v>-374962.91000000015</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A77" t="s">
         <v>38</v>
       </c>
@@ -5652,7 +5680,7 @@
         <v>-72.879999999888241</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A78" t="s">
         <v>39</v>
       </c>
@@ -5681,7 +5709,7 @@
         <v>-1724.9000000000233</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A79" t="s">
         <v>55</v>
       </c>
@@ -5708,6 +5736,9 @@
       <c r="G79">
         <f t="shared" si="10"/>
         <v>-82077.349999999627</v>
+      </c>
+      <c r="K79" s="9" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.5">

</xml_diff>